<commit_message>
Added density depth relationships
</commit_message>
<xml_diff>
--- a/docs/Examples/Ne_Line_Fitting/Ne_Lines_fit_loop.xlsx
+++ b/docs/Examples/Ne_Line_Fitting/Ne_Lines_fit_loop.xlsx
@@ -489,22 +489,22 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1448.004552684449</v>
+        <v>1448.004569101116</v>
       </c>
       <c r="D2">
-        <v>0.00804</v>
+        <v>0.00722</v>
       </c>
       <c r="E2">
         <v>1117.594044392368</v>
       </c>
       <c r="G2">
-        <v>330.4105082920807</v>
+        <v>330.410524708748</v>
       </c>
       <c r="H2">
-        <v>1.000203158514135</v>
+        <v>1.000203039801087</v>
       </c>
       <c r="K2">
-        <v>162.3584184550459</v>
+        <v>141.256915563747</v>
       </c>
       <c r="L2">
         <v>1080.953924223215</v>
@@ -518,22 +518,22 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1448.001120544332</v>
+        <v>1448.001134958084</v>
       </c>
       <c r="D3">
-        <v>0.00804</v>
+        <v>0.00723</v>
       </c>
       <c r="E3">
         <v>1117.811820515916</v>
       </c>
       <c r="G3">
-        <v>330.1893000284163</v>
+        <v>330.1893144421676</v>
       </c>
       <c r="H3">
-        <v>1.000873238386462</v>
+        <v>1.000873125631825</v>
       </c>
       <c r="K3">
-        <v>157.5922465564901</v>
+        <v>136.6455115309842</v>
       </c>
       <c r="L3">
         <v>11.98437035272926</v>
@@ -547,22 +547,22 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1448.020910562887</v>
+        <v>1448.020926302389</v>
       </c>
       <c r="D4">
-        <v>0.00781</v>
+        <v>0.00702</v>
       </c>
       <c r="E4">
         <v>1117.833297606049</v>
       </c>
       <c r="G4">
-        <v>330.1876129568373</v>
+        <v>330.1876286963393</v>
       </c>
       <c r="H4">
-        <v>1.000878352281497</v>
+        <v>1.000878235507392</v>
       </c>
       <c r="K4">
-        <v>153.9367213700891</v>
+        <v>133.3476666884557</v>
       </c>
       <c r="L4">
         <v>12.82306096606991</v>
@@ -576,22 +576,22 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1448.005148160575</v>
+        <v>1448.11284983611</v>
       </c>
       <c r="D5">
-        <v>0.008189999999999999</v>
+        <v>0.014</v>
       </c>
       <c r="E5">
         <v>1117.807916604986</v>
       </c>
       <c r="G5">
-        <v>330.197231555589</v>
+        <v>330.3049332311246</v>
       </c>
       <c r="H5">
-        <v>1.000849196836357</v>
+        <v>1.00052278348721</v>
       </c>
       <c r="K5">
-        <v>160.3105815422042</v>
+        <v>231.059180373549</v>
       </c>
       <c r="L5">
         <v>12.82309433399354</v>
@@ -605,22 +605,22 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>1447.991178121054</v>
+        <v>1447.991191605644</v>
       </c>
       <c r="D6">
-        <v>0.008319999999999999</v>
+        <v>0.00747</v>
       </c>
       <c r="E6">
         <v>1117.803325208428</v>
       </c>
       <c r="G6">
-        <v>330.1878529126259</v>
+        <v>330.1878663972166</v>
       </c>
       <c r="H6">
-        <v>1.000877624918112</v>
+        <v>1.000877514979296</v>
       </c>
       <c r="K6">
-        <v>156.2345525909114</v>
+        <v>135.593271084326</v>
       </c>
       <c r="L6">
         <v>15.41211098124478</v>
@@ -634,22 +634,22 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>1448.031285593424</v>
+        <v>1448.031301948534</v>
       </c>
       <c r="D7">
-        <v>0.00738</v>
+        <v>0.00663</v>
       </c>
       <c r="E7">
         <v>1117.84096406065</v>
       </c>
       <c r="G7">
-        <v>330.1903215327736</v>
+        <v>330.190337887884</v>
       </c>
       <c r="H7">
-        <v>1.000870142001415</v>
+        <v>1.000870023362632</v>
       </c>
       <c r="K7">
-        <v>145.5544007985566</v>
+        <v>126.639645308679</v>
       </c>
       <c r="L7">
         <v>14.34768161339439</v>
@@ -663,22 +663,22 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1448.0245934646</v>
+        <v>1448.024610067631</v>
       </c>
       <c r="D8">
-        <v>0.00787</v>
+        <v>0.00707</v>
       </c>
       <c r="E8">
         <v>1117.825607652814</v>
       </c>
       <c r="G8">
-        <v>330.1989858117863</v>
+        <v>330.199002414817</v>
       </c>
       <c r="H8">
-        <v>1.000843879600444</v>
+        <v>1.00084376021462</v>
       </c>
       <c r="K8">
-        <v>159.9017390885321</v>
+        <v>139.141402826869</v>
       </c>
       <c r="L8">
         <v>13.79276673590751</v>
@@ -692,22 +692,22 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>1448.034860209692</v>
+        <v>1448.034876468905</v>
       </c>
       <c r="D9">
-        <v>0.00717</v>
+        <v>0.00645</v>
       </c>
       <c r="E9">
         <v>1117.846137736414</v>
       </c>
       <c r="G9">
-        <v>330.1887224732777</v>
+        <v>330.1887387324909</v>
       </c>
       <c r="H9">
-        <v>1.000874989080663</v>
+        <v>1.000874870731751</v>
       </c>
       <c r="K9">
-        <v>140.0297123837476</v>
+        <v>121.9973720959166</v>
       </c>
       <c r="L9">
         <v>14.86813559853819</v>
@@ -721,22 +721,22 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>1448.029855710009</v>
+        <v>1448.029871734082</v>
       </c>
       <c r="D10">
-        <v>0.00752</v>
+        <v>0.00676</v>
       </c>
       <c r="E10">
         <v>1117.849656666884</v>
       </c>
       <c r="G10">
-        <v>330.180199043125</v>
+        <v>330.1802150671983</v>
       </c>
       <c r="H10">
-        <v>1.000900826148076</v>
+        <v>1.000900708507634</v>
       </c>
       <c r="K10">
-        <v>147.199838383778</v>
+        <v>128.0108410899661</v>
       </c>
       <c r="L10">
         <v>13.71787527125299</v>
@@ -750,22 +750,22 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>1448.02490078332</v>
+        <v>1448.024917666296</v>
       </c>
       <c r="D11">
-        <v>0.00788</v>
+        <v>0.00708</v>
       </c>
       <c r="E11">
         <v>1117.835268722676</v>
       </c>
       <c r="G11">
-        <v>330.1896320606443</v>
+        <v>330.1896489436203</v>
       </c>
       <c r="H11">
-        <v>1.000872231927933</v>
+        <v>1.00087211168873</v>
       </c>
       <c r="K11">
-        <v>154.6041541643658</v>
+        <v>134.6010612846933</v>
       </c>
       <c r="L11">
         <v>11.310499457523</v>
@@ -779,22 +779,22 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>1448.022239127118</v>
+        <v>1448.022255336594</v>
       </c>
       <c r="D12">
-        <v>0.00749</v>
+        <v>0.00673</v>
       </c>
       <c r="E12">
         <v>1117.832725050401</v>
       </c>
       <c r="G12">
-        <v>330.1895140767169</v>
+        <v>330.1895302861935</v>
       </c>
       <c r="H12">
-        <v>1.000872589561449</v>
+        <v>1.0008724713637</v>
       </c>
       <c r="K12">
-        <v>144.7660424635041</v>
+        <v>125.9009063268143</v>
       </c>
       <c r="L12">
         <v>13.23520795115999</v>
@@ -808,22 +808,22 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>1448.017413887748</v>
+        <v>1448.017430005813</v>
       </c>
       <c r="D13">
-        <v>0.007900000000000001</v>
+        <v>0.0071</v>
       </c>
       <c r="E13">
         <v>1117.832456676811</v>
       </c>
       <c r="G13">
-        <v>330.1849572109372</v>
+        <v>330.1849733290023</v>
       </c>
       <c r="H13">
-        <v>1.000886402553087</v>
+        <v>1.000886284630124</v>
       </c>
       <c r="K13">
-        <v>156.1827005200318</v>
+        <v>135.9233781216712</v>
       </c>
       <c r="L13">
         <v>13.13772877370966</v>

</xml_diff>